<commit_message>
Fixed typo labeling "Active Learning" group as "Process"
</commit_message>
<xml_diff>
--- a/stratified_latent_profile_analysis/outputs_option2/latent_profile_analysis_5_clusters.xlsx
+++ b/stratified_latent_profile_analysis/outputs_option2/latent_profile_analysis_5_clusters.xlsx
@@ -13652,7 +13652,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Process</t>
+          <t>Active Learning</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -14003,7 +14003,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Process</t>
+          <t>Active Learning</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -14354,7 +14354,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Process</t>
+          <t>Active Learning</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -14715,7 +14715,7 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Process</t>
+          <t>Active Learning</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">

</xml_diff>